<commit_message>
diagrama de negocio e especificacao do log
</commit_message>
<xml_diff>
--- a/Documentação do Projeto/especificacao-funcional-estruturada.xlsx
+++ b/Documentação do Projeto/especificacao-funcional-estruturada.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27628"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{160CB915-FF35-4C70-819F-B871634F675C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E98230AF-F469-400F-AC0A-60A11E4A1213}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Especificações</t>
   </si>
@@ -174,12 +174,21 @@
 	Estabelecimento de um plano de backup e recuperação para garantir a integridade e disponibilidade dos dados.
 	Utilização de banco de dados relacional ou NoSQL, conforme a natureza dos dados e requisitos de desempenho.</t>
   </si>
+  <si>
+    <t>Log - erro de login</t>
+  </si>
+  <si>
+    <t>Registra cada tentativa de login falha, incluindo data e hora do evento, arquitetura da máquina, sistema operacional, e a mensagem de erro.</t>
+  </si>
+  <si>
+    <t>Verifica as credenciais fornecidas com as armazenadas no banco de dados, se não forem as mesmas será criado um aquivo txt   através da aplicação java. Será criado um arquivo txt por dia, o nome será o ano, mês e dia, do dia criado.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <name val="Arial"/>
@@ -219,6 +228,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -270,7 +286,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -284,40 +300,37 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="4">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="3" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="6" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="5">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="3" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="6" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="4" applyFont="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -334,9 +347,19 @@
   </cellStyles>
   <dxfs count="8">
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
       </font>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
     </dxf>
     <dxf>
       <font>
@@ -369,16 +392,6 @@
         <top/>
         <bottom/>
       </border>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="1" hidden="0"/>
     </dxf>
     <dxf>
@@ -459,9 +472,9 @@
     <filterColumn colId="2" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Requisito" totalsRowLabel="Total" totalsRowDxfId="1" dataCellStyle="Normal"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Funcional " totalsRowDxfId="3" dataCellStyle="Responsável"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Técnica" totalsRowFunction="count" dataDxfId="0" totalsRowDxfId="2" dataCellStyle="Data"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Requisito" totalsRowLabel="Total" totalsRowDxfId="3" dataCellStyle="Normal"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Funcional " totalsRowDxfId="2" dataCellStyle="Responsável"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Técnica" totalsRowFunction="count" dataDxfId="1" totalsRowDxfId="0" dataCellStyle="Data"/>
   </tableColumns>
   <tableStyleInfo name="Lista de verificação do Plano de Negócios" showFirstColumn="0" showLastColumn="1" showRowStripes="0" showColumnStripes="1"/>
   <extLst>
@@ -765,8 +778,8 @@
   </sheetPr>
   <dimension ref="B1:D18"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -774,7 +787,7 @@
     <col min="1" max="1" width="2.59765625" customWidth="1"/>
     <col min="2" max="2" width="26.8984375" customWidth="1"/>
     <col min="3" max="3" width="40.19921875" customWidth="1"/>
-    <col min="4" max="4" width="41" style="13" customWidth="1"/>
+    <col min="4" max="4" width="41" customWidth="1"/>
     <col min="5" max="5" width="2.59765625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -787,119 +800,125 @@
       </c>
     </row>
     <row r="3" spans="2:4" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
+      <c r="B3" s="14"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
     </row>
     <row r="4" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="8" t="s">
         <v>1</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="15" t="s">
+      <c r="D4" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="2:4" s="7" customFormat="1" ht="110.4" x14ac:dyDescent="0.25">
-      <c r="B5" s="12" t="s">
+    <row r="5" spans="2:4" s="6" customFormat="1" ht="96.6" x14ac:dyDescent="0.25">
+      <c r="B5" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="11" t="s">
+      <c r="D5" s="10" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="2:4" ht="165.6" x14ac:dyDescent="0.25">
-      <c r="B6" s="8" t="s">
+    <row r="6" spans="2:4" ht="151.80000000000001" x14ac:dyDescent="0.25">
+      <c r="B6" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="11" t="s">
+      <c r="D6" s="10" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="7" spans="2:4" ht="179.4" x14ac:dyDescent="0.25">
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="11" t="s">
+      <c r="D7" s="10" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="8" spans="2:4" ht="110.4" x14ac:dyDescent="0.25">
-      <c r="B8" s="12" t="s">
+      <c r="B8" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="16" t="s">
+      <c r="D8" s="13" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="9" spans="2:4" ht="165.6" x14ac:dyDescent="0.25">
-      <c r="B9" s="12" t="s">
+      <c r="B9" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="11" t="s">
+      <c r="D9" s="10" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="10" spans="2:4" ht="138" x14ac:dyDescent="0.25">
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D10" s="11" t="s">
+      <c r="D10" s="10" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B11" s="16"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="11"/>
+    <row r="11" spans="2:4" ht="82.8" x14ac:dyDescent="0.25">
+      <c r="B11" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C12" s="3"/>
-      <c r="D12" s="14"/>
+      <c r="D12" s="12"/>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C13" s="3"/>
-      <c r="D13" s="14"/>
+      <c r="D13" s="12"/>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C14" s="3"/>
-      <c r="D14" s="14"/>
+      <c r="D14" s="12"/>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C15" s="3"/>
-      <c r="D15" s="14"/>
+      <c r="D15" s="12"/>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C16" s="3"/>
-      <c r="D16" s="14"/>
+      <c r="D16" s="12"/>
     </row>
     <row r="17" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C17" s="3"/>
-      <c r="D17" s="14"/>
+      <c r="D17" s="12"/>
     </row>
     <row r="18" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C18" s="3"/>
-      <c r="D18" s="14"/>
+      <c r="D18" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -927,6 +946,35 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </Image>
+    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
+    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </ImageTagsTaxHTField>
+    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
+    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010079F111ED35F8CC479449609E8A0923A6" ma:contentTypeVersion="26" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ac37c1753acd5e330d2062ccec26ea66">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xmlns:ns3="16c05727-aa75-4e4a-9b5f-8a80a1165891" xmlns:ns4="230e9df3-be65-4c73-a93b-d1236ebd677e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3b340c7101c92c5120abd06486f94548" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -1226,36 +1274,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </Image>
-    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
-    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </ImageTagsTaxHTField>
-    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
-    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E4994F8E-3141-47F3-91B7-8A348AFEAE97}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9B3E0A64-3B79-40D0-B5B8-9F6FE2202932}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
+    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3A16C7A7-3246-4EB4-B7D0-9FB37D6AB99A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1276,26 +1315,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9B3E0A64-3B79-40D0-B5B8-9F6FE2202932}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
-    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E4994F8E-3141-47F3-91B7-8A348AFEAE97}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata"/>
 </file>
</xml_diff>